<commit_message>
Create New Document From The Portal
</commit_message>
<xml_diff>
--- a/eInvoicing.Web/Content/Uploads/ORO TAX WS 9-2021-V4.xlsx
+++ b/eInvoicing.Web/Content/Uploads/ORO TAX WS 9-2021-V4.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB59B11-1C68-43B9-83F6-3F1406815443}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4921D300-2A80-4232-8725-D67F808C901F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documents" sheetId="1" r:id="rId1"/>
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BE3" sqref="BE3"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>